<commit_message>
Updated the Monthy Change Charge formula due to a mistake
</commit_message>
<xml_diff>
--- a/AWS_Backup_Costs.xlsx
+++ b/AWS_Backup_Costs.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://shiandms-my.sharepoint.com/personal/clinton_davenport_shi_com/Documents/Personal/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tools\Code\AWS Backup Costs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="34" documentId="8_{21703378-2A2A-AC4E-B877-934927D9E7FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B507040-4B59-4B06-82D8-E50AD877FF15}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB8CD557-5861-4AEE-82BB-81B9D436E887}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="330" windowWidth="33510" windowHeight="22425" xr2:uid="{CB5E2608-74ED-804E-986F-6D4A353708E7}"/>
   </bookViews>
@@ -638,27 +638,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -684,6 +663,27 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="4" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -1003,7 +1003,7 @@
   <dimension ref="A1:G48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="G44" sqref="G44"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1019,10 +1019,10 @@
   <sheetData>
     <row r="1" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:7" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="31"/>
+      <c r="B2" s="42"/>
     </row>
     <row r="3" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
@@ -1075,12 +1075,12 @@
     </row>
     <row r="9" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:7" ht="21.75" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="26"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="27"/>
+      <c r="B10" s="37"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="38"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
@@ -1090,8 +1090,8 @@
         <f>(IN_DCR*IN_Disk_Size)/IN_Snaps_per_Day</f>
         <v>10.24</v>
       </c>
-      <c r="C11" s="28"/>
-      <c r="D11" s="29"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="40"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
@@ -1101,10 +1101,10 @@
         <f>IN_Disk_Size*IN_DCR</f>
         <v>10.24</v>
       </c>
-      <c r="C12" s="37" t="s">
+      <c r="C12" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="38" t="s">
+      <c r="D12" s="31" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1139,33 +1139,33 @@
         <v>418.83046439425033</v>
       </c>
       <c r="C14" s="22">
-        <f>(B14/30)*IN_Backup_PPG</f>
-        <v>0.69805077399041726</v>
+        <f>((IN_Backup_Retention_Daily/30)*B14)*IN_Backup_PPG</f>
+        <v>4.8863554179329212</v>
       </c>
       <c r="D14" s="23">
         <f>B13+C14</f>
-        <v>26.298050773990418</v>
+        <v>30.486355417932923</v>
       </c>
       <c r="E14" s="24"/>
     </row>
     <row r="15" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:7" ht="32.25" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="34" t="s">
+      <c r="B16" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="34" t="s">
+      <c r="C16" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="34" t="s">
+      <c r="D16" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="E16" s="35" t="s">
+      <c r="E16" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="F16" s="36" t="s">
+      <c r="F16" s="29" t="s">
         <v>20</v>
       </c>
       <c r="G16" s="3"/>
@@ -1187,11 +1187,11 @@
         <v>10.242244383561644</v>
       </c>
       <c r="E17" s="7">
-        <f>D17*IN_Snaps_per_Day*IN_Backup_Retention_Daily</f>
+        <f t="shared" ref="E17:E46" si="2">D17*IN_Snaps_per_Day*IN_Backup_Retention_Daily</f>
         <v>71.695710684931512</v>
       </c>
       <c r="F17" s="8">
-        <f>E17/30*IN_Backup_PPG</f>
+        <f t="shared" ref="F17:F46" si="3">E17/30*IN_Backup_PPG</f>
         <v>0.11949285114155253</v>
       </c>
       <c r="G17" s="1"/>
@@ -1213,11 +1213,11 @@
         <v>10.244489259042973</v>
       </c>
       <c r="E18" s="7">
-        <f>D18*IN_Snaps_per_Day*IN_Backup_Retention_Daily</f>
+        <f t="shared" si="2"/>
         <v>71.711424813300809</v>
       </c>
       <c r="F18" s="8">
-        <f>E18/30*IN_Backup_PPG</f>
+        <f t="shared" si="3"/>
         <v>0.11951904135550136</v>
       </c>
       <c r="G18" s="1"/>
@@ -1227,7 +1227,7 @@
         <v>3</v>
       </c>
       <c r="B19" s="7">
-        <f t="shared" ref="B19:B46" si="2">IN_Disk_Size*(IN_AGR/365)+B18</f>
+        <f t="shared" ref="B19:B46" si="4">IN_Disk_Size*(IN_AGR/365)+B18</f>
         <v>512.33668213023088</v>
       </c>
       <c r="C19" s="7">
@@ -1239,11 +1239,11 @@
         <v>10.246733642604617</v>
       </c>
       <c r="E19" s="7">
-        <f>D19*IN_Snaps_per_Day*IN_Backup_Retention_Daily</f>
+        <f t="shared" si="2"/>
         <v>71.727135498232315</v>
       </c>
       <c r="F19" s="8">
-        <f>E19/30*IN_Backup_PPG</f>
+        <f t="shared" si="3"/>
         <v>0.11954522583038718</v>
       </c>
       <c r="G19" s="1"/>
@@ -1253,7 +1253,7 @@
         <v>4</v>
       </c>
       <c r="B20" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>512.44890130831311</v>
       </c>
       <c r="C20" s="7">
@@ -1265,11 +1265,11 @@
         <v>10.248978026166263</v>
       </c>
       <c r="E20" s="7">
-        <f>D20*IN_Snaps_per_Day*IN_Backup_Retention_Daily</f>
+        <f t="shared" si="2"/>
         <v>71.742846183163834</v>
       </c>
       <c r="F20" s="8">
-        <f>E20/30*IN_Backup_PPG</f>
+        <f t="shared" si="3"/>
         <v>0.11957141030527306</v>
       </c>
       <c r="G20" s="1"/>
@@ -1279,7 +1279,7 @@
         <v>5</v>
       </c>
       <c r="B21" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>512.56112048639534</v>
       </c>
       <c r="C21" s="7">
@@ -1291,11 +1291,11 @@
         <v>10.251222409727907</v>
       </c>
       <c r="E21" s="7">
-        <f>D21*IN_Snaps_per_Day*IN_Backup_Retention_Daily</f>
+        <f t="shared" si="2"/>
         <v>71.758556868095354</v>
       </c>
       <c r="F21" s="8">
-        <f>E21/30*IN_Backup_PPG</f>
+        <f t="shared" si="3"/>
         <v>0.11959759478015893</v>
       </c>
       <c r="G21" s="1"/>
@@ -1305,7 +1305,7 @@
         <v>6</v>
       </c>
       <c r="B22" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>512.67333966447757</v>
       </c>
       <c r="C22" s="7">
@@ -1317,11 +1317,11 @@
         <v>10.253466793289551</v>
       </c>
       <c r="E22" s="7">
-        <f>D22*IN_Snaps_per_Day*IN_Backup_Retention_Daily</f>
+        <f t="shared" si="2"/>
         <v>71.77426755302686</v>
       </c>
       <c r="F22" s="8">
-        <f>E22/30*IN_Backup_PPG</f>
+        <f t="shared" si="3"/>
         <v>0.11962377925504478</v>
       </c>
       <c r="G22" s="1"/>
@@ -1331,7 +1331,7 @@
         <v>7</v>
       </c>
       <c r="B23" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>512.78555884255979</v>
       </c>
       <c r="C23" s="7">
@@ -1343,11 +1343,11 @@
         <v>10.255711176851197</v>
       </c>
       <c r="E23" s="7">
-        <f>D23*IN_Snaps_per_Day*IN_Backup_Retention_Daily</f>
+        <f t="shared" si="2"/>
         <v>71.78997823795838</v>
       </c>
       <c r="F23" s="8">
-        <f>E23/30*IN_Backup_PPG</f>
+        <f t="shared" si="3"/>
         <v>0.11964996372993064</v>
       </c>
       <c r="G23" s="1"/>
@@ -1357,7 +1357,7 @@
         <v>8</v>
       </c>
       <c r="B24" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>512.89777802064202</v>
       </c>
       <c r="C24" s="7">
@@ -1369,11 +1369,11 @@
         <v>10.257955560412841</v>
       </c>
       <c r="E24" s="7">
-        <f>D24*IN_Snaps_per_Day*IN_Backup_Retention_Daily</f>
+        <f t="shared" si="2"/>
         <v>71.805688922889885</v>
       </c>
       <c r="F24" s="8">
-        <f>E24/30*IN_Backup_PPG</f>
+        <f t="shared" si="3"/>
         <v>0.11967614820481648</v>
       </c>
       <c r="G24" s="1"/>
@@ -1383,7 +1383,7 @@
         <v>9</v>
       </c>
       <c r="B25" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>513.00999719872425</v>
       </c>
       <c r="C25" s="7">
@@ -1395,11 +1395,11 @@
         <v>10.260199943974484</v>
       </c>
       <c r="E25" s="7">
-        <f>D25*IN_Snaps_per_Day*IN_Backup_Retention_Daily</f>
+        <f t="shared" si="2"/>
         <v>71.821399607821391</v>
       </c>
       <c r="F25" s="8">
-        <f>E25/30*IN_Backup_PPG</f>
+        <f t="shared" si="3"/>
         <v>0.11970233267970232</v>
       </c>
       <c r="G25" s="1"/>
@@ -1409,7 +1409,7 @@
         <v>10</v>
       </c>
       <c r="B26" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>513.12221637680648</v>
       </c>
       <c r="C26" s="7">
@@ -1421,11 +1421,11 @@
         <v>10.26244432753613</v>
       </c>
       <c r="E26" s="7">
-        <f>D26*IN_Snaps_per_Day*IN_Backup_Retention_Daily</f>
+        <f t="shared" si="2"/>
         <v>71.837110292752911</v>
       </c>
       <c r="F26" s="8">
-        <f>E26/30*IN_Backup_PPG</f>
+        <f t="shared" si="3"/>
         <v>0.1197285171545882</v>
       </c>
       <c r="G26" s="1"/>
@@ -1435,7 +1435,7 @@
         <v>11</v>
       </c>
       <c r="B27" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>513.23443555488871</v>
       </c>
       <c r="C27" s="7">
@@ -1447,11 +1447,11 @@
         <v>10.264688711097774</v>
       </c>
       <c r="E27" s="7">
-        <f>D27*IN_Snaps_per_Day*IN_Backup_Retention_Daily</f>
+        <f t="shared" si="2"/>
         <v>71.852820977684416</v>
       </c>
       <c r="F27" s="8">
-        <f>E27/30*IN_Backup_PPG</f>
+        <f t="shared" si="3"/>
         <v>0.11975470162947405</v>
       </c>
       <c r="G27" s="1"/>
@@ -1461,7 +1461,7 @@
         <v>12</v>
       </c>
       <c r="B28" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>513.34665473297093</v>
       </c>
       <c r="C28" s="7">
@@ -1473,11 +1473,11 @@
         <v>10.26693309465942</v>
       </c>
       <c r="E28" s="7">
-        <f>D28*IN_Snaps_per_Day*IN_Backup_Retention_Daily</f>
+        <f t="shared" si="2"/>
         <v>71.868531662615936</v>
       </c>
       <c r="F28" s="8">
-        <f>E28/30*IN_Backup_PPG</f>
+        <f t="shared" si="3"/>
         <v>0.11978088610435988</v>
       </c>
       <c r="G28" s="1"/>
@@ -1487,7 +1487,7 @@
         <v>13</v>
       </c>
       <c r="B29" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>513.45887391105316</v>
       </c>
       <c r="C29" s="7">
@@ -1499,11 +1499,11 @@
         <v>10.269177478221064</v>
       </c>
       <c r="E29" s="7">
-        <f>D29*IN_Snaps_per_Day*IN_Backup_Retention_Daily</f>
+        <f t="shared" si="2"/>
         <v>71.884242347547442</v>
       </c>
       <c r="F29" s="8">
-        <f>E29/30*IN_Backup_PPG</f>
+        <f t="shared" si="3"/>
         <v>0.11980707057924574</v>
       </c>
       <c r="G29" s="1"/>
@@ -1513,7 +1513,7 @@
         <v>14</v>
       </c>
       <c r="B30" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>513.57109308913539</v>
       </c>
       <c r="C30" s="7">
@@ -1525,11 +1525,11 @@
         <v>10.271421861782708</v>
       </c>
       <c r="E30" s="7">
-        <f>D30*IN_Snaps_per_Day*IN_Backup_Retention_Daily</f>
+        <f t="shared" si="2"/>
         <v>71.899953032478948</v>
       </c>
       <c r="F30" s="8">
-        <f>E30/30*IN_Backup_PPG</f>
+        <f t="shared" si="3"/>
         <v>0.11983325505413159</v>
       </c>
       <c r="G30" s="1"/>
@@ -1539,7 +1539,7 @@
         <v>15</v>
       </c>
       <c r="B31" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>513.68331226721762</v>
       </c>
       <c r="C31" s="7">
@@ -1551,11 +1551,11 @@
         <v>10.273666245344353</v>
       </c>
       <c r="E31" s="7">
-        <f>D31*IN_Snaps_per_Day*IN_Backup_Retention_Daily</f>
+        <f t="shared" si="2"/>
         <v>71.915663717410467</v>
       </c>
       <c r="F31" s="8">
-        <f>E31/30*IN_Backup_PPG</f>
+        <f t="shared" si="3"/>
         <v>0.11985943952901745</v>
       </c>
       <c r="G31" s="1"/>
@@ -1565,7 +1565,7 @@
         <v>16</v>
       </c>
       <c r="B32" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>513.79553144529984</v>
       </c>
       <c r="C32" s="7">
@@ -1577,11 +1577,11 @@
         <v>10.275910628905997</v>
       </c>
       <c r="E32" s="7">
-        <f>D32*IN_Snaps_per_Day*IN_Backup_Retention_Daily</f>
+        <f t="shared" si="2"/>
         <v>71.931374402341987</v>
       </c>
       <c r="F32" s="8">
-        <f>E32/30*IN_Backup_PPG</f>
+        <f t="shared" si="3"/>
         <v>0.1198856240039033</v>
       </c>
       <c r="G32" s="1"/>
@@ -1591,7 +1591,7 @@
         <v>17</v>
       </c>
       <c r="B33" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>513.90775062338207</v>
       </c>
       <c r="C33" s="7">
@@ -1603,11 +1603,11 @@
         <v>10.278155012467641</v>
       </c>
       <c r="E33" s="7">
-        <f>D33*IN_Snaps_per_Day*IN_Backup_Retention_Daily</f>
+        <f t="shared" si="2"/>
         <v>71.947085087273493</v>
       </c>
       <c r="F33" s="8">
-        <f>E33/30*IN_Backup_PPG</f>
+        <f t="shared" si="3"/>
         <v>0.11991180847878916</v>
       </c>
       <c r="G33" s="1"/>
@@ -1617,7 +1617,7 @@
         <v>18</v>
       </c>
       <c r="B34" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>514.0199698014643</v>
       </c>
       <c r="C34" s="7">
@@ -1629,11 +1629,11 @@
         <v>10.280399396029287</v>
       </c>
       <c r="E34" s="7">
-        <f>D34*IN_Snaps_per_Day*IN_Backup_Retention_Daily</f>
+        <f t="shared" si="2"/>
         <v>71.962795772205013</v>
       </c>
       <c r="F34" s="8">
-        <f>E34/30*IN_Backup_PPG</f>
+        <f t="shared" si="3"/>
         <v>0.11993799295367502</v>
       </c>
       <c r="G34" s="1"/>
@@ -1643,7 +1643,7 @@
         <v>19</v>
       </c>
       <c r="B35" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>514.13218897954653</v>
       </c>
       <c r="C35" s="7">
@@ -1655,11 +1655,11 @@
         <v>10.282643779590931</v>
       </c>
       <c r="E35" s="7">
-        <f>D35*IN_Snaps_per_Day*IN_Backup_Retention_Daily</f>
+        <f t="shared" si="2"/>
         <v>71.978506457136518</v>
       </c>
       <c r="F35" s="8">
-        <f>E35/30*IN_Backup_PPG</f>
+        <f t="shared" si="3"/>
         <v>0.11996417742856087</v>
       </c>
       <c r="G35" s="1"/>
@@ -1669,7 +1669,7 @@
         <v>20</v>
       </c>
       <c r="B36" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>514.24440815762875</v>
       </c>
       <c r="C36" s="7">
@@ -1681,11 +1681,11 @@
         <v>10.284888163152575</v>
       </c>
       <c r="E36" s="7">
-        <f>D36*IN_Snaps_per_Day*IN_Backup_Retention_Daily</f>
+        <f t="shared" si="2"/>
         <v>71.994217142068024</v>
       </c>
       <c r="F36" s="8">
-        <f>E36/30*IN_Backup_PPG</f>
+        <f t="shared" si="3"/>
         <v>0.1199903619034467</v>
       </c>
       <c r="G36" s="1"/>
@@ -1695,7 +1695,7 @@
         <v>21</v>
       </c>
       <c r="B37" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>514.35662733571098</v>
       </c>
       <c r="C37" s="7">
@@ -1707,11 +1707,11 @@
         <v>10.28713254671422</v>
       </c>
       <c r="E37" s="7">
-        <f>D37*IN_Snaps_per_Day*IN_Backup_Retention_Daily</f>
+        <f t="shared" si="2"/>
         <v>72.009927826999544</v>
       </c>
       <c r="F37" s="8">
-        <f>E37/30*IN_Backup_PPG</f>
+        <f t="shared" si="3"/>
         <v>0.12001654637833258</v>
       </c>
       <c r="G37" s="1"/>
@@ -1721,7 +1721,7 @@
         <v>22</v>
       </c>
       <c r="B38" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>514.46884651379321</v>
       </c>
       <c r="C38" s="7">
@@ -1733,11 +1733,11 @@
         <v>10.289376930275864</v>
       </c>
       <c r="E38" s="7">
-        <f>D38*IN_Snaps_per_Day*IN_Backup_Retention_Daily</f>
+        <f t="shared" si="2"/>
         <v>72.025638511931049</v>
       </c>
       <c r="F38" s="8">
-        <f>E38/30*IN_Backup_PPG</f>
+        <f t="shared" si="3"/>
         <v>0.12004273085321843</v>
       </c>
       <c r="G38" s="1"/>
@@ -1747,7 +1747,7 @@
         <v>23</v>
       </c>
       <c r="B39" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>514.58106569187544</v>
       </c>
       <c r="C39" s="7">
@@ -1759,11 +1759,11 @@
         <v>10.291621313837508</v>
       </c>
       <c r="E39" s="7">
-        <f>D39*IN_Snaps_per_Day*IN_Backup_Retention_Daily</f>
+        <f t="shared" si="2"/>
         <v>72.041349196862555</v>
       </c>
       <c r="F39" s="8">
-        <f>E39/30*IN_Backup_PPG</f>
+        <f t="shared" si="3"/>
         <v>0.12006891532810426</v>
       </c>
       <c r="G39" s="1"/>
@@ -1773,7 +1773,7 @@
         <v>24</v>
       </c>
       <c r="B40" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>514.69328486995767</v>
       </c>
       <c r="C40" s="7">
@@ -1785,11 +1785,11 @@
         <v>10.293865697399154</v>
       </c>
       <c r="E40" s="7">
-        <f>D40*IN_Snaps_per_Day*IN_Backup_Retention_Daily</f>
+        <f t="shared" si="2"/>
         <v>72.057059881794075</v>
       </c>
       <c r="F40" s="8">
-        <f>E40/30*IN_Backup_PPG</f>
+        <f t="shared" si="3"/>
         <v>0.12009509980299014</v>
       </c>
       <c r="G40" s="1"/>
@@ -1799,7 +1799,7 @@
         <v>25</v>
       </c>
       <c r="B41" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>514.80550404803989</v>
       </c>
       <c r="C41" s="7">
@@ -1811,11 +1811,11 @@
         <v>10.296110080960798</v>
       </c>
       <c r="E41" s="7">
-        <f>D41*IN_Snaps_per_Day*IN_Backup_Retention_Daily</f>
+        <f t="shared" si="2"/>
         <v>72.07277056672558</v>
       </c>
       <c r="F41" s="8">
-        <f>E41/30*IN_Backup_PPG</f>
+        <f t="shared" si="3"/>
         <v>0.12012128427787597</v>
       </c>
       <c r="G41" s="1"/>
@@ -1825,7 +1825,7 @@
         <v>26</v>
       </c>
       <c r="B42" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>514.91772322612212</v>
       </c>
       <c r="C42" s="7">
@@ -1837,11 +1837,11 @@
         <v>10.298354464522443</v>
       </c>
       <c r="E42" s="7">
-        <f>D42*IN_Snaps_per_Day*IN_Backup_Retention_Daily</f>
+        <f t="shared" si="2"/>
         <v>72.0884812516571</v>
       </c>
       <c r="F42" s="8">
-        <f>E42/30*IN_Backup_PPG</f>
+        <f t="shared" si="3"/>
         <v>0.12014746875276183</v>
       </c>
       <c r="G42" s="1"/>
@@ -1851,7 +1851,7 @@
         <v>27</v>
       </c>
       <c r="B43" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>515.02994240420435</v>
       </c>
       <c r="C43" s="7">
@@ -1863,11 +1863,11 @@
         <v>10.300598848084087</v>
       </c>
       <c r="E43" s="7">
-        <f>D43*IN_Snaps_per_Day*IN_Backup_Retention_Daily</f>
+        <f t="shared" si="2"/>
         <v>72.104191936588606</v>
       </c>
       <c r="F43" s="8">
-        <f>E43/30*IN_Backup_PPG</f>
+        <f t="shared" si="3"/>
         <v>0.12017365322764768</v>
       </c>
       <c r="G43" s="1"/>
@@ -1877,7 +1877,7 @@
         <v>28</v>
       </c>
       <c r="B44" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>515.14216158228658</v>
       </c>
       <c r="C44" s="7">
@@ -1889,11 +1889,11 @@
         <v>10.302843231645731</v>
       </c>
       <c r="E44" s="7">
-        <f>D44*IN_Snaps_per_Day*IN_Backup_Retention_Daily</f>
+        <f t="shared" si="2"/>
         <v>72.119902621520112</v>
       </c>
       <c r="F44" s="8">
-        <f>E44/30*IN_Backup_PPG</f>
+        <f t="shared" si="3"/>
         <v>0.12019983770253354</v>
       </c>
       <c r="G44" s="1"/>
@@ -1903,7 +1903,7 @@
         <v>29</v>
       </c>
       <c r="B45" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>515.2543807603688</v>
       </c>
       <c r="C45" s="7">
@@ -1915,11 +1915,11 @@
         <v>10.305087615207377</v>
       </c>
       <c r="E45" s="7">
-        <f>D45*IN_Snaps_per_Day*IN_Backup_Retention_Daily</f>
+        <f t="shared" si="2"/>
         <v>72.135613306451631</v>
       </c>
       <c r="F45" s="8">
-        <f>E45/30*IN_Backup_PPG</f>
+        <f t="shared" si="3"/>
         <v>0.12022602217741939</v>
       </c>
       <c r="G45" s="1"/>
@@ -1929,7 +1929,7 @@
         <v>30</v>
       </c>
       <c r="B46" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>515.36659993845103</v>
       </c>
       <c r="C46" s="11">
@@ -1941,44 +1941,44 @@
         <v>10.307331998769021</v>
       </c>
       <c r="E46" s="7">
-        <f>D46*IN_Snaps_per_Day*IN_Backup_Retention_Daily</f>
+        <f t="shared" si="2"/>
         <v>72.151323991383151</v>
       </c>
       <c r="F46" s="8">
-        <f>E46/30*IN_Backup_PPG</f>
+        <f t="shared" si="3"/>
         <v>0.12025220665230525</v>
       </c>
       <c r="G46" s="1"/>
     </row>
     <row r="47" spans="1:7" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="39" t="s">
+      <c r="A47" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="B47" s="40">
-        <f t="shared" ref="B47:D47" si="3">SUM(B17:B46)</f>
+      <c r="B47" s="33">
+        <f t="shared" ref="B47:D47" si="5">SUM(B17:B46)</f>
         <v>15412.182631091779</v>
       </c>
-      <c r="C47" s="40">
-        <f t="shared" si="3"/>
+      <c r="C47" s="33">
+        <f t="shared" si="5"/>
         <v>52.182631091777694</v>
       </c>
-      <c r="D47" s="40">
-        <f t="shared" si="3"/>
+      <c r="D47" s="33">
+        <f t="shared" si="5"/>
         <v>308.24365262183551</v>
       </c>
-      <c r="E47" s="40">
+      <c r="E47" s="33">
         <f>SUM(E17:E46)</f>
         <v>2157.7055683528488</v>
       </c>
-      <c r="F47" s="41">
+      <c r="F47" s="34">
         <f>SUM(F17:F46)</f>
         <v>3.5961759472547481</v>
       </c>
       <c r="G47" s="4"/>
     </row>
     <row r="48" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="E48" s="32"/>
-      <c r="F48" s="42"/>
+      <c r="E48" s="25"/>
+      <c r="F48" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>